<commit_message>
Outbound Costs done, Excel files updated
</commit_message>
<xml_diff>
--- a/Outbound.xlsx
+++ b/Outbound.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bff73b0ba30a6b9/Dokumen/College Files/OR/OR8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_30EFB159AC1B5F3C0B675960D0F62E0BFB9F52F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3533A59E-6E28-4BEC-AB26-8795F827B8E9}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="11_30EFB159AC1B5F3C0B675960D0F62E0BFB9F52F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{289E12BE-A3E2-41DF-AE7D-B86CD9D0E74F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="__AIMMS_SETUP__" sheetId="6" state="veryHidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Transport Outbound DC'!$A$1:$K$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Transport Outbound DC'!$B$1:$L$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>CA</t>
   </si>
@@ -99,6 +99,132 @@
   </si>
   <si>
     <t xml:space="preserve">$7 </t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NH</t>
+  </si>
+  <si>
+    <t>NJ</t>
+  </si>
+  <si>
+    <t>NM</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>RI</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VT</t>
+  </si>
+  <si>
+    <t>WI</t>
+  </si>
+  <si>
+    <t>WV</t>
+  </si>
+  <si>
+    <t>WY</t>
+  </si>
+  <si>
+    <t>DC</t>
   </si>
 </sst>
 </file>
@@ -109,7 +235,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -134,6 +260,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -274,7 +406,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -325,14 +457,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -351,6 +492,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -622,167 +767,179 @@
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="9" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="I54" sqref="I54"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" customWidth="1"/>
-    <col min="10" max="10" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" customWidth="1"/>
+    <col min="11" max="11" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="6" customWidth="1"/>
     <col min="16" max="16" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="K1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="13">
-        <v>7</v>
-      </c>
-      <c r="B2" s="19">
-        <v>0.40539999999999998</v>
+      <c r="A2" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="13">
+        <v>7</v>
       </c>
       <c r="C2" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="D2" s="19">
-        <v>0.1754</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="E2" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.1754</v>
       </c>
       <c r="F2" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="G2" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="H2" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I2" s="19">
-        <v>0.3105</v>
+        <v>0.2631</v>
       </c>
       <c r="J2" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.3105</v>
       </c>
       <c r="K2" s="19">
         <v>0.40539999999999998</v>
       </c>
+      <c r="L2" s="19">
+        <v>0.40539999999999998</v>
+      </c>
     </row>
     <row r="3" spans="1:19" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14">
-        <v>7</v>
-      </c>
-      <c r="B3" s="19">
-        <v>0.2036</v>
+      <c r="A3" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="14">
+        <v>7</v>
       </c>
       <c r="C3" s="19">
-        <v>0.1754</v>
+        <v>0.2036</v>
       </c>
       <c r="D3" s="19">
-        <v>0.3105</v>
+        <v>0.1754</v>
       </c>
       <c r="E3" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.3105</v>
       </c>
       <c r="F3" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G3" s="19">
-        <v>0.2631</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="H3" s="19">
         <v>0.2631</v>
       </c>
       <c r="I3" s="19">
-        <v>0.3105</v>
+        <v>0.2631</v>
       </c>
       <c r="J3" s="19">
-        <v>0.1754</v>
+        <v>0.3105</v>
       </c>
       <c r="K3" s="19">
+        <v>0.1754</v>
+      </c>
+      <c r="L3" s="19">
         <v>5.67E-2</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="14">
-        <v>7</v>
-      </c>
-      <c r="B4" s="19">
-        <v>0.2036</v>
+      <c r="A4" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="14">
+        <v>7</v>
       </c>
       <c r="C4" s="19">
-        <v>0.1754</v>
+        <v>0.2036</v>
       </c>
       <c r="D4" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
       </c>
       <c r="E4" s="19">
-        <v>0.3105</v>
+        <v>0.2631</v>
       </c>
       <c r="F4" s="19">
-        <v>5.67E-2</v>
+        <v>0.3105</v>
       </c>
       <c r="G4" s="19">
-        <v>0.2631</v>
+        <v>5.67E-2</v>
       </c>
       <c r="H4" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="I4" s="19">
-        <v>0.2631</v>
+        <v>0.2036</v>
       </c>
       <c r="J4" s="19">
-        <v>5.67E-2</v>
+        <v>0.2631</v>
       </c>
       <c r="K4" s="19">
+        <v>5.67E-2</v>
+      </c>
+      <c r="L4" s="19">
         <v>5.67E-2</v>
       </c>
       <c r="Q4" s="10"/>
@@ -790,37 +947,40 @@
       <c r="S4" s="9"/>
     </row>
     <row r="5" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="14">
-        <v>7</v>
-      </c>
-      <c r="B5" s="19">
-        <v>0.40539999999999998</v>
+      <c r="A5" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="14">
+        <v>7</v>
       </c>
       <c r="C5" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="D5" s="19">
-        <v>0.1754</v>
+        <v>0.3105</v>
       </c>
       <c r="E5" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
       </c>
       <c r="F5" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="G5" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="H5" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I5" s="19">
-        <v>0.2631</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="J5" s="19">
-        <v>0.1754</v>
+        <v>0.2631</v>
       </c>
       <c r="K5" s="19">
+        <v>0.1754</v>
+      </c>
+      <c r="L5" s="19">
         <v>0.2036</v>
       </c>
       <c r="Q5" s="10"/>
@@ -828,37 +988,40 @@
       <c r="S5" s="9"/>
     </row>
     <row r="6" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="14">
-        <v>7</v>
-      </c>
-      <c r="B6" s="19">
-        <v>0.40539999999999998</v>
+      <c r="A6" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="14">
+        <v>7</v>
       </c>
       <c r="C6" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="D6" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.3105</v>
       </c>
       <c r="E6" s="19">
-        <v>0.2036</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="F6" s="19">
-        <v>0.2631</v>
+        <v>0.2036</v>
       </c>
       <c r="G6" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2631</v>
       </c>
       <c r="H6" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I6" s="19">
-        <v>0.3105</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="J6" s="19">
-        <v>0.2036</v>
+        <v>0.3105</v>
       </c>
       <c r="K6" s="19">
+        <v>0.2036</v>
+      </c>
+      <c r="L6" s="19">
         <v>0.2631</v>
       </c>
       <c r="Q6" s="10"/>
@@ -866,37 +1029,40 @@
       <c r="S6" s="9"/>
     </row>
     <row r="7" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="14">
-        <v>7</v>
-      </c>
-      <c r="B7" s="19">
-        <v>0.3105</v>
+      <c r="A7" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="14">
+        <v>7</v>
       </c>
       <c r="C7" s="19">
-        <v>0.2036</v>
+        <v>0.3105</v>
       </c>
       <c r="D7" s="19">
         <v>0.2036</v>
       </c>
       <c r="E7" s="19">
-        <v>0.2631</v>
+        <v>0.2036</v>
       </c>
       <c r="F7" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.2631</v>
       </c>
       <c r="G7" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="H7" s="19">
-        <v>5.67E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I7" s="19">
-        <v>0.1754</v>
+        <v>5.67E-2</v>
       </c>
       <c r="J7" s="19">
-        <v>5.67E-2</v>
+        <v>0.1754</v>
       </c>
       <c r="K7" s="19">
+        <v>5.67E-2</v>
+      </c>
+      <c r="L7" s="19">
         <v>0.1754</v>
       </c>
       <c r="Q7" s="10"/>
@@ -904,17 +1070,17 @@
       <c r="S7" s="9"/>
     </row>
     <row r="8" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="14">
-        <v>7</v>
-      </c>
-      <c r="B8" s="19">
-        <v>9.8500000000000004E-2</v>
+      <c r="A8" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="14">
+        <v>7</v>
       </c>
       <c r="C8" s="19">
-        <v>0.2036</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="D8" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="E8" s="19">
         <v>0.40539999999999998</v>
@@ -923,18 +1089,21 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="G8" s="19">
-        <v>5.67E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H8" s="19">
-        <v>0.40539999999999998</v>
+        <v>5.67E-2</v>
       </c>
       <c r="I8" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="J8" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K8" s="19">
+        <v>0.3105</v>
+      </c>
+      <c r="L8" s="19">
         <v>0.2036</v>
       </c>
       <c r="Q8" s="10"/>
@@ -942,17 +1111,17 @@
       <c r="S8" s="9"/>
     </row>
     <row r="9" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="14">
-        <v>7</v>
-      </c>
-      <c r="B9" s="19">
-        <v>9.8500000000000004E-2</v>
+      <c r="A9" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="14">
+        <v>7</v>
       </c>
       <c r="C9" s="19">
-        <v>0.2036</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="D9" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="E9" s="19">
         <v>0.40539999999999998</v>
@@ -961,18 +1130,21 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="G9" s="19">
-        <v>5.67E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H9" s="19">
-        <v>0.40539999999999998</v>
+        <v>5.67E-2</v>
       </c>
       <c r="I9" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="J9" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K9" s="19">
+        <v>0.3105</v>
+      </c>
+      <c r="L9" s="19">
         <v>0.1754</v>
       </c>
       <c r="Q9" s="10"/>
@@ -980,37 +1152,40 @@
       <c r="S9" s="9"/>
     </row>
     <row r="10" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="14">
-        <v>7</v>
-      </c>
-      <c r="B10" s="19">
-        <v>0.2036</v>
+      <c r="A10" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="14">
+        <v>7</v>
       </c>
       <c r="C10" s="19">
         <v>0.2036</v>
       </c>
       <c r="D10" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="E10" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="F10" s="19">
-        <v>0.2036</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G10" s="19">
         <v>0.2036</v>
       </c>
       <c r="H10" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="I10" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="J10" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K10" s="19">
+        <v>0.2631</v>
+      </c>
+      <c r="L10" s="19">
         <v>0.13930000000000001</v>
       </c>
       <c r="Q10" s="10"/>
@@ -1018,46 +1193,49 @@
       <c r="S10" s="9"/>
     </row>
     <row r="11" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="14">
-        <v>7</v>
-      </c>
-      <c r="B11" s="19">
-        <v>0.2036</v>
+      <c r="A11" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="14">
+        <v>7</v>
       </c>
       <c r="C11" s="19">
-        <v>0.1754</v>
+        <v>0.2036</v>
       </c>
       <c r="D11" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.1754</v>
       </c>
       <c r="E11" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="F11" s="19">
-        <v>0.2036</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G11" s="19">
         <v>0.2036</v>
       </c>
       <c r="H11" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="I11" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="J11" s="19">
-        <v>0.2036</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K11" s="19">
+        <v>0.2036</v>
+      </c>
+      <c r="L11" s="19">
         <v>5.67E-2</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="14">
-        <v>7</v>
-      </c>
-      <c r="B12" s="19">
-        <v>0.40539999999999998</v>
+      <c r="A12" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="14">
+        <v>7</v>
       </c>
       <c r="C12" s="19">
         <v>0.40539999999999998</v>
@@ -1086,264 +1264,288 @@
       <c r="K12" s="19">
         <v>0.40539999999999998</v>
       </c>
+      <c r="L12" s="19">
+        <v>0.40539999999999998</v>
+      </c>
     </row>
     <row r="13" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="14">
-        <v>7</v>
-      </c>
-      <c r="B13" s="19">
-        <v>0.2036</v>
+      <c r="A13" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="14">
+        <v>7</v>
       </c>
       <c r="C13" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.2036</v>
       </c>
       <c r="D13" s="19">
-        <v>0.2631</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="E13" s="19">
-        <v>0.3105</v>
+        <v>0.2631</v>
       </c>
       <c r="F13" s="19">
-        <v>0.1754</v>
+        <v>0.3105</v>
       </c>
       <c r="G13" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
       </c>
       <c r="H13" s="19">
-        <v>0.1754</v>
+        <v>0.2631</v>
       </c>
       <c r="I13" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.1754</v>
       </c>
       <c r="J13" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="K13" s="19">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L13" s="19">
         <v>0.13930000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="14">
-        <v>7</v>
-      </c>
-      <c r="B14" s="19">
-        <v>0.40539999999999998</v>
+      <c r="A14" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="14">
+        <v>7</v>
       </c>
       <c r="C14" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="D14" s="19">
-        <v>0.2036</v>
+        <v>0.3105</v>
       </c>
       <c r="E14" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.2036</v>
       </c>
       <c r="F14" s="19">
-        <v>0.40539999999999998</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="G14" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="H14" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I14" s="19">
-        <v>0.13930000000000001</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="J14" s="19">
-        <v>0.1754</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="K14" s="19">
+        <v>0.1754</v>
+      </c>
+      <c r="L14" s="19">
         <v>0.2631</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="14">
-        <v>7</v>
-      </c>
-      <c r="B15" s="19">
-        <v>0.2036</v>
+      <c r="A15" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="14">
+        <v>7</v>
       </c>
       <c r="C15" s="19">
-        <v>5.67E-2</v>
+        <v>0.2036</v>
       </c>
       <c r="D15" s="19">
-        <v>0.3105</v>
+        <v>5.67E-2</v>
       </c>
       <c r="E15" s="19">
         <v>0.3105</v>
       </c>
       <c r="F15" s="19">
-        <v>0.2036</v>
+        <v>0.3105</v>
       </c>
       <c r="G15" s="19">
-        <v>0.1754</v>
+        <v>0.2036</v>
       </c>
       <c r="H15" s="19">
-        <v>0.2036</v>
+        <v>0.1754</v>
       </c>
       <c r="I15" s="19">
         <v>0.2036</v>
       </c>
       <c r="J15" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.2036</v>
       </c>
       <c r="K15" s="19">
         <v>9.8500000000000004E-2</v>
       </c>
+      <c r="L15" s="19">
+        <v>9.8500000000000004E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="14">
-        <v>7</v>
-      </c>
-      <c r="B16" s="19">
-        <v>0.1754</v>
+      <c r="A16" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="14">
+        <v>7</v>
       </c>
       <c r="C16" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.1754</v>
       </c>
       <c r="D16" s="19">
-        <v>0.3105</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="E16" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.3105</v>
       </c>
       <c r="F16" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G16" s="19">
-        <v>0.1754</v>
+        <v>0.2631</v>
       </c>
       <c r="H16" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
       </c>
       <c r="I16" s="19">
-        <v>5.67E-2</v>
+        <v>0.2631</v>
       </c>
       <c r="J16" s="19">
-        <v>0.13930000000000001</v>
+        <v>5.67E-2</v>
       </c>
       <c r="K16" s="19">
-        <v>9.8500000000000004E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="14">
-        <v>7</v>
-      </c>
-      <c r="B17" s="19">
-        <v>0.2631</v>
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="L16" s="19">
+        <v>9.8500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="14">
+        <v>7</v>
       </c>
       <c r="C17" s="19">
-        <v>0.1754</v>
+        <v>0.2631</v>
       </c>
       <c r="D17" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
       </c>
       <c r="E17" s="19">
-        <v>0.3105</v>
+        <v>0.2631</v>
       </c>
       <c r="F17" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.3105</v>
       </c>
       <c r="G17" s="19">
-        <v>0.3105</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="H17" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.3105</v>
       </c>
       <c r="I17" s="19">
-        <v>0.1754</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="J17" s="19">
-        <v>5.67E-2</v>
+        <v>0.1754</v>
       </c>
       <c r="K17" s="19">
         <v>5.67E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="14">
-        <v>7</v>
-      </c>
-      <c r="B18" s="19">
-        <v>0.1754</v>
+      <c r="L17" s="19">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="14">
+        <v>7</v>
       </c>
       <c r="C18" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.1754</v>
       </c>
       <c r="D18" s="19">
-        <v>0.3105</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="E18" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.3105</v>
       </c>
       <c r="F18" s="19">
-        <v>0.1754</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G18" s="19">
         <v>0.1754</v>
       </c>
       <c r="H18" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
       </c>
       <c r="I18" s="19">
         <v>0.2631</v>
       </c>
       <c r="J18" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.2631</v>
       </c>
       <c r="K18" s="19">
-        <v>5.67E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="14">
-        <v>7</v>
-      </c>
-      <c r="B19" s="19">
-        <v>0.2631</v>
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="L18" s="19">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="14">
+        <v>7</v>
       </c>
       <c r="C19" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="D19" s="19">
-        <v>0.3105</v>
+        <v>0.2036</v>
       </c>
       <c r="E19" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.3105</v>
       </c>
       <c r="F19" s="19">
-        <v>5.67E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G19" s="19">
-        <v>0.40539999999999998</v>
+        <v>5.67E-2</v>
       </c>
       <c r="H19" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I19" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2631</v>
       </c>
       <c r="J19" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K19" s="19">
         <v>0.13930000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="14">
-        <v>7</v>
-      </c>
-      <c r="B20" s="19">
-        <v>0.13930000000000001</v>
+      <c r="L19" s="19">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="14">
+        <v>7</v>
       </c>
       <c r="C20" s="19">
-        <v>0.2036</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="D20" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="E20" s="19">
         <v>0.40539999999999998</v>
@@ -1352,33 +1554,36 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="G20" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H20" s="19">
-        <v>0.40539999999999998</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="I20" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="J20" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K20" s="19">
-        <v>0.2036</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="14">
-        <v>7</v>
-      </c>
-      <c r="B21" s="19">
-        <v>5.67E-2</v>
+        <v>0.3105</v>
+      </c>
+      <c r="L20" s="19">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="14">
+        <v>7</v>
       </c>
       <c r="C21" s="19">
-        <v>0.13930000000000001</v>
+        <v>5.67E-2</v>
       </c>
       <c r="D21" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="E21" s="19">
         <v>0.40539999999999998</v>
@@ -1387,33 +1592,36 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="G21" s="19">
-        <v>5.67E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H21" s="19">
-        <v>0.40539999999999998</v>
+        <v>5.67E-2</v>
       </c>
       <c r="I21" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="J21" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K21" s="19">
-        <v>0.13930000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="14">
-        <v>7</v>
-      </c>
-      <c r="B22" s="19">
-        <v>0.1754</v>
+        <v>0.3105</v>
+      </c>
+      <c r="L21" s="19">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="14">
+        <v>7</v>
       </c>
       <c r="C22" s="19">
-        <v>0.2036</v>
+        <v>0.1754</v>
       </c>
       <c r="D22" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="E22" s="19">
         <v>0.40539999999999998</v>
@@ -1422,10 +1630,10 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="G22" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H22" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="I22" s="19">
         <v>0.40539999999999998</v>
@@ -1436,19 +1644,22 @@
       <c r="K22" s="19">
         <v>0.40539999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="14">
-        <v>7</v>
-      </c>
-      <c r="B23" s="19">
-        <v>0.1754</v>
+      <c r="L22" s="19">
+        <v>0.40539999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="14">
+        <v>7</v>
       </c>
       <c r="C23" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.1754</v>
       </c>
       <c r="D23" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="E23" s="19">
         <v>0.40539999999999998</v>
@@ -1457,278 +1668,302 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="G23" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H23" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2631</v>
       </c>
       <c r="I23" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="J23" s="19">
-        <v>0.1754</v>
+        <v>0.2631</v>
       </c>
       <c r="K23" s="19">
         <v>0.1754</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="14">
-        <v>7</v>
-      </c>
-      <c r="B24" s="19">
-        <v>0.2036</v>
+      <c r="L23" s="19">
+        <v>0.1754</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="14">
+        <v>7</v>
       </c>
       <c r="C24" s="19">
-        <v>0.1754</v>
+        <v>0.2036</v>
       </c>
       <c r="D24" s="19">
-        <v>0.3105</v>
+        <v>0.1754</v>
       </c>
       <c r="E24" s="19">
-        <v>0.2631</v>
+        <v>0.3105</v>
       </c>
       <c r="F24" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2631</v>
       </c>
       <c r="G24" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H24" s="19">
         <v>0.2631</v>
       </c>
       <c r="I24" s="19">
-        <v>0.1754</v>
+        <v>0.2631</v>
       </c>
       <c r="J24" s="19">
         <v>0.1754</v>
       </c>
       <c r="K24" s="19">
-        <v>0.2036</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="14">
-        <v>7</v>
-      </c>
-      <c r="B25" s="19">
-        <v>0.2036</v>
+        <v>0.1754</v>
+      </c>
+      <c r="L24" s="19">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="14">
+        <v>7</v>
       </c>
       <c r="C25" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.2036</v>
       </c>
       <c r="D25" s="19">
-        <v>0.3105</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="E25" s="19">
         <v>0.3105</v>
       </c>
       <c r="F25" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.3105</v>
       </c>
       <c r="G25" s="19">
-        <v>0.2036</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="H25" s="19">
-        <v>0.1754</v>
+        <v>0.2036</v>
       </c>
       <c r="I25" s="19">
-        <v>0.2036</v>
+        <v>0.1754</v>
       </c>
       <c r="J25" s="19">
-        <v>5.67E-2</v>
+        <v>0.2036</v>
       </c>
       <c r="K25" s="19">
         <v>5.67E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="14">
-        <v>7</v>
-      </c>
-      <c r="B26" s="19">
-        <v>0.2036</v>
+      <c r="L25" s="19">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="14">
+        <v>7</v>
       </c>
       <c r="C26" s="19">
         <v>0.2036</v>
       </c>
       <c r="D26" s="19">
-        <v>0.3105</v>
+        <v>0.2036</v>
       </c>
       <c r="E26" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.3105</v>
       </c>
       <c r="F26" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G26" s="19">
-        <v>0.2631</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="H26" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="I26" s="19">
-        <v>0.3105</v>
+        <v>0.2036</v>
       </c>
       <c r="J26" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.3105</v>
       </c>
       <c r="K26" s="19">
-        <v>5.67E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="14">
-        <v>7</v>
-      </c>
-      <c r="B27" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="L26" s="19">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="14">
+        <v>7</v>
       </c>
       <c r="C27" s="19">
-        <v>0.2036</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="D27" s="19">
-        <v>0.1754</v>
+        <v>0.2036</v>
       </c>
       <c r="E27" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.1754</v>
       </c>
       <c r="F27" s="19">
-        <v>0.40539999999999998</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="G27" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="H27" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I27" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="J27" s="19">
-        <v>0.1754</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="K27" s="19">
-        <v>0.40539999999999998</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="14">
-        <v>7</v>
-      </c>
-      <c r="B28" s="19">
-        <v>0.1754</v>
+        <v>0.1754</v>
+      </c>
+      <c r="L27" s="19">
+        <v>0.40539999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="14">
+        <v>7</v>
       </c>
       <c r="C28" s="19">
         <v>0.1754</v>
       </c>
       <c r="D28" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.1754</v>
       </c>
       <c r="E28" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="F28" s="19">
-        <v>0.1754</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G28" s="19">
         <v>0.1754</v>
       </c>
       <c r="H28" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.1754</v>
       </c>
       <c r="I28" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="J28" s="19">
-        <v>0.2036</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K28" s="19">
-        <v>5.67E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="14">
-        <v>7</v>
-      </c>
-      <c r="B29" s="19">
-        <v>0.2631</v>
+        <v>0.2036</v>
+      </c>
+      <c r="L28" s="19">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="14">
+        <v>7</v>
       </c>
       <c r="C29" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="D29" s="19">
-        <v>0.2631</v>
+        <v>0.2036</v>
       </c>
       <c r="E29" s="19">
         <v>0.2631</v>
       </c>
       <c r="F29" s="19">
-        <v>0.3105</v>
+        <v>0.2631</v>
       </c>
       <c r="G29" s="19">
         <v>0.3105</v>
       </c>
       <c r="H29" s="19">
-        <v>0.2036</v>
+        <v>0.3105</v>
       </c>
       <c r="I29" s="19">
-        <v>5.67E-2</v>
+        <v>0.2036</v>
       </c>
       <c r="J29" s="19">
-        <v>0.1754</v>
+        <v>5.67E-2</v>
       </c>
       <c r="K29" s="19">
-        <v>0.2036</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="14">
-        <v>7</v>
-      </c>
-      <c r="B30" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
+      </c>
+      <c r="L29" s="19">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="14">
+        <v>7</v>
       </c>
       <c r="C30" s="19">
-        <v>0.1754</v>
+        <v>0.2631</v>
       </c>
       <c r="D30" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
       </c>
       <c r="E30" s="19">
         <v>0.2631</v>
       </c>
       <c r="F30" s="19">
-        <v>0.1754</v>
+        <v>0.2631</v>
       </c>
       <c r="G30" s="19">
-        <v>0.3105</v>
+        <v>0.1754</v>
       </c>
       <c r="H30" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.3105</v>
       </c>
       <c r="I30" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="J30" s="19">
-        <v>5.67E-2</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="K30" s="19">
-        <v>0.13930000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="14">
-        <v>7</v>
-      </c>
-      <c r="B31" s="19">
-        <v>0.13930000000000001</v>
+        <v>5.67E-2</v>
+      </c>
+      <c r="L30" s="19">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="14">
+        <v>7</v>
       </c>
       <c r="C31" s="19">
-        <v>0.2036</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="D31" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="E31" s="19">
         <v>0.40539999999999998</v>
@@ -1737,33 +1972,36 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="G31" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H31" s="19">
-        <v>0.40539999999999998</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="I31" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="J31" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K31" s="19">
-        <v>0.2631</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="14">
-        <v>7</v>
-      </c>
-      <c r="B32" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.3105</v>
+      </c>
+      <c r="L31" s="19">
+        <v>0.2631</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="14">
+        <v>7</v>
       </c>
       <c r="C32" s="19">
-        <v>0.2036</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="D32" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="E32" s="19">
         <v>0.40539999999999998</v>
@@ -1772,103 +2010,112 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="G32" s="19">
-        <v>5.67E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H32" s="19">
-        <v>0.40539999999999998</v>
+        <v>5.67E-2</v>
       </c>
       <c r="I32" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="J32" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K32" s="19">
-        <v>0.2036</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="14">
-        <v>7</v>
-      </c>
-      <c r="B33" s="19">
-        <v>0.3105</v>
+        <v>0.3105</v>
+      </c>
+      <c r="L32" s="19">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="14">
+        <v>7</v>
       </c>
       <c r="C33" s="19">
-        <v>0.2631</v>
+        <v>0.3105</v>
       </c>
       <c r="D33" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="E33" s="19">
-        <v>0.2631</v>
+        <v>0.2036</v>
       </c>
       <c r="F33" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.2631</v>
       </c>
       <c r="G33" s="19">
-        <v>0.40539999999999998</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="H33" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I33" s="19">
-        <v>0.2631</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="J33" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.2631</v>
       </c>
       <c r="K33" s="19">
-        <v>0.1754</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="14">
-        <v>7</v>
-      </c>
-      <c r="B34" s="19">
-        <v>0.40539999999999998</v>
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L33" s="19">
+        <v>0.1754</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="14">
+        <v>7</v>
       </c>
       <c r="C34" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="D34" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.3105</v>
       </c>
       <c r="E34" s="19">
-        <v>0.2036</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="F34" s="19">
         <v>0.2036</v>
       </c>
       <c r="G34" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="H34" s="19">
-        <v>5.67E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I34" s="19">
-        <v>0.2036</v>
+        <v>5.67E-2</v>
       </c>
       <c r="J34" s="19">
-        <v>0.1754</v>
+        <v>0.2036</v>
       </c>
       <c r="K34" s="19">
-        <v>0.3105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="14">
-        <v>7</v>
-      </c>
-      <c r="B35" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.1754</v>
+      </c>
+      <c r="L34" s="19">
+        <v>0.3105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="14">
+        <v>7</v>
       </c>
       <c r="C35" s="19">
-        <v>0.2036</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="D35" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="E35" s="19">
         <v>0.40539999999999998</v>
@@ -1877,173 +2124,188 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="G35" s="19">
-        <v>5.67E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H35" s="19">
-        <v>0.40539999999999998</v>
+        <v>5.67E-2</v>
       </c>
       <c r="I35" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="J35" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K35" s="19">
-        <v>0.2631</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="14">
-        <v>7</v>
-      </c>
-      <c r="B36" s="19">
-        <v>0.1754</v>
+        <v>0.3105</v>
+      </c>
+      <c r="L35" s="19">
+        <v>0.2631</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="14">
+        <v>7</v>
       </c>
       <c r="C36" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.1754</v>
       </c>
       <c r="D36" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="E36" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="F36" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G36" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.2631</v>
       </c>
       <c r="H36" s="19">
-        <v>0.2631</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="I36" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="J36" s="19">
-        <v>0.1754</v>
+        <v>0.2036</v>
       </c>
       <c r="K36" s="19">
-        <v>9.8500000000000004E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="14">
-        <v>7</v>
-      </c>
-      <c r="B37" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
+      </c>
+      <c r="L36" s="19">
+        <v>9.8500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="14">
+        <v>7</v>
       </c>
       <c r="C37" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="D37" s="19">
-        <v>0.2631</v>
+        <v>0.2036</v>
       </c>
       <c r="E37" s="19">
-        <v>0.3105</v>
+        <v>0.2631</v>
       </c>
       <c r="F37" s="19">
-        <v>5.67E-2</v>
+        <v>0.3105</v>
       </c>
       <c r="G37" s="19">
-        <v>0.3105</v>
+        <v>5.67E-2</v>
       </c>
       <c r="H37" s="19">
-        <v>0.1754</v>
+        <v>0.3105</v>
       </c>
       <c r="I37" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
       </c>
       <c r="J37" s="19">
-        <v>5.67E-2</v>
+        <v>0.2631</v>
       </c>
       <c r="K37" s="19">
-        <v>9.8500000000000004E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="14">
-        <v>7</v>
-      </c>
-      <c r="B38" s="19">
-        <v>0.40539999999999998</v>
+        <v>5.67E-2</v>
+      </c>
+      <c r="L37" s="19">
+        <v>9.8500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="14">
+        <v>7</v>
       </c>
       <c r="C38" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="D38" s="19">
-        <v>0.2036</v>
+        <v>0.3105</v>
       </c>
       <c r="E38" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.2036</v>
       </c>
       <c r="F38" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="G38" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="H38" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I38" s="19">
-        <v>0.1754</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="J38" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
       </c>
       <c r="K38" s="19">
-        <v>0.40539999999999998</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="14">
-        <v>7</v>
-      </c>
-      <c r="B39" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.2631</v>
+      </c>
+      <c r="L38" s="19">
+        <v>0.40539999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="14">
+        <v>7</v>
       </c>
       <c r="C39" s="19">
-        <v>0.1754</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="D39" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.1754</v>
       </c>
       <c r="E39" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="F39" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G39" s="19">
         <v>0.2631</v>
       </c>
       <c r="H39" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="I39" s="19">
-        <v>0.2631</v>
+        <v>0.2036</v>
       </c>
       <c r="J39" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.2631</v>
       </c>
       <c r="K39" s="19">
         <v>0.13930000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="14">
-        <v>7</v>
-      </c>
-      <c r="B40" s="19">
-        <v>0.13930000000000001</v>
+      <c r="L39" s="19">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="14">
+        <v>7</v>
       </c>
       <c r="C40" s="19">
-        <v>0.2036</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="D40" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="E40" s="19">
         <v>0.40539999999999998</v>
@@ -2052,10 +2314,10 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="G40" s="19">
-        <v>5.67E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H40" s="19">
-        <v>0.40539999999999998</v>
+        <v>5.67E-2</v>
       </c>
       <c r="I40" s="19">
         <v>0.40539999999999998</v>
@@ -2064,231 +2326,252 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="K40" s="19">
-        <v>0.2036</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="14">
-        <v>7</v>
-      </c>
-      <c r="B41" s="19">
-        <v>0.1754</v>
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="L40" s="19">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="14">
+        <v>7</v>
       </c>
       <c r="C41" s="19">
-        <v>0.2036</v>
+        <v>0.1754</v>
       </c>
       <c r="D41" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="E41" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="F41" s="19">
-        <v>0.1754</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G41" s="19">
-        <v>0.2036</v>
+        <v>0.1754</v>
       </c>
       <c r="H41" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="I41" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="J41" s="19">
-        <v>0.1754</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K41" s="19">
-        <v>5.67E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="14">
-        <v>7</v>
-      </c>
-      <c r="B42" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
+      </c>
+      <c r="L41" s="19">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="14">
+        <v>7</v>
       </c>
       <c r="C42" s="19">
-        <v>0.1754</v>
+        <v>0.2631</v>
       </c>
       <c r="D42" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
       </c>
       <c r="E42" s="19">
         <v>0.2631</v>
       </c>
       <c r="F42" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="G42" s="19">
-        <v>0.2631</v>
+        <v>0.2036</v>
       </c>
       <c r="H42" s="19">
-        <v>0.1754</v>
+        <v>0.2631</v>
       </c>
       <c r="I42" s="19">
-        <v>5.67E-2</v>
+        <v>0.1754</v>
       </c>
       <c r="J42" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>5.67E-2</v>
       </c>
       <c r="K42" s="19">
-        <v>0.1754</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="14">
-        <v>7</v>
-      </c>
-      <c r="B43" s="19">
-        <v>0.2036</v>
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L42" s="19">
+        <v>0.1754</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="14">
+        <v>7</v>
       </c>
       <c r="C43" s="19">
-        <v>0.1754</v>
+        <v>0.2036</v>
       </c>
       <c r="D43" s="19">
-        <v>0.3105</v>
+        <v>0.1754</v>
       </c>
       <c r="E43" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.3105</v>
       </c>
       <c r="F43" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G43" s="19">
-        <v>0.1754</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="H43" s="19">
-        <v>0.2631</v>
+        <v>0.1754</v>
       </c>
       <c r="I43" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="J43" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.2036</v>
       </c>
       <c r="K43" s="19">
         <v>9.8500000000000004E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="14">
-        <v>7</v>
-      </c>
-      <c r="B44" s="19">
-        <v>0.2631</v>
+      <c r="L43" s="19">
+        <v>9.8500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="14">
+        <v>7</v>
       </c>
       <c r="C44" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="D44" s="19">
-        <v>0.2631</v>
+        <v>0.2036</v>
       </c>
       <c r="E44" s="19">
-        <v>0.3105</v>
+        <v>0.2631</v>
       </c>
       <c r="F44" s="19">
-        <v>5.67E-2</v>
+        <v>0.3105</v>
       </c>
       <c r="G44" s="19">
-        <v>0.40539999999999998</v>
+        <v>5.67E-2</v>
       </c>
       <c r="H44" s="19">
-        <v>0.1754</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I44" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.1754</v>
       </c>
       <c r="J44" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K44" s="19">
-        <v>0.13930000000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="14">
-        <v>7</v>
-      </c>
-      <c r="B45" s="19">
-        <v>0.40539999999999998</v>
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L44" s="19">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="14">
+        <v>7</v>
       </c>
       <c r="C45" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="D45" s="19">
-        <v>0.1754</v>
+        <v>0.2631</v>
       </c>
       <c r="E45" s="19">
-        <v>0.2036</v>
+        <v>0.1754</v>
       </c>
       <c r="F45" s="19">
-        <v>0.3105</v>
+        <v>0.2036</v>
       </c>
       <c r="G45" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.3105</v>
       </c>
       <c r="H45" s="19">
-        <v>5.67E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I45" s="19">
-        <v>0.1754</v>
+        <v>5.67E-2</v>
       </c>
       <c r="J45" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.1754</v>
       </c>
       <c r="K45" s="19">
-        <v>0.13930000000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="14">
-        <v>7</v>
-      </c>
-      <c r="B46" s="19">
-        <v>0.13930000000000001</v>
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L45" s="19">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="14">
+        <v>7</v>
       </c>
       <c r="C46" s="19">
-        <v>0.1754</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="D46" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.1754</v>
       </c>
       <c r="E46" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="F46" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G46" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.2631</v>
       </c>
       <c r="H46" s="19">
-        <v>0.40539999999999998</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="I46" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="J46" s="19">
-        <v>0.1754</v>
+        <v>0.3105</v>
       </c>
       <c r="K46" s="19">
-        <v>5.67E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="14">
-        <v>7</v>
-      </c>
-      <c r="B47" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.1754</v>
+      </c>
+      <c r="L46" s="19">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="14">
+        <v>7</v>
       </c>
       <c r="C47" s="19">
-        <v>0.2036</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="D47" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="E47" s="19">
         <v>0.40539999999999998</v>
@@ -2297,10 +2580,10 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="G47" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H47" s="19">
-        <v>0.40539999999999998</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="I47" s="19">
         <v>0.40539999999999998</v>
@@ -2309,123 +2592,135 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="K47" s="19">
-        <v>0.3105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="14">
-        <v>7</v>
-      </c>
-      <c r="B48" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.40539999999999998</v>
+      </c>
+      <c r="L47" s="19">
+        <v>0.3105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="14">
+        <v>7</v>
       </c>
       <c r="C48" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="D48" s="19">
-        <v>0.2036</v>
+        <v>0.3105</v>
       </c>
       <c r="E48" s="19">
-        <v>5.67E-2</v>
+        <v>0.2036</v>
       </c>
       <c r="F48" s="19">
-        <v>0.40539999999999998</v>
+        <v>5.67E-2</v>
       </c>
       <c r="G48" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="H48" s="19">
-        <v>0.1754</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I48" s="19">
         <v>0.1754</v>
       </c>
       <c r="J48" s="19">
-        <v>0.3105</v>
+        <v>0.1754</v>
       </c>
       <c r="K48" s="19">
-        <v>0.40539999999999998</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="14">
-        <v>7</v>
-      </c>
-      <c r="B49" s="19">
-        <v>0.2036</v>
+        <v>0.3105</v>
+      </c>
+      <c r="L48" s="19">
+        <v>0.40539999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" s="14">
+        <v>7</v>
       </c>
       <c r="C49" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.2036</v>
       </c>
       <c r="D49" s="19">
-        <v>0.3105</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="E49" s="19">
         <v>0.3105</v>
       </c>
       <c r="F49" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.3105</v>
       </c>
       <c r="G49" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H49" s="19">
-        <v>0.2036</v>
+        <v>0.2631</v>
       </c>
       <c r="I49" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>0.2036</v>
       </c>
       <c r="J49" s="19">
-        <v>0.13930000000000001</v>
+        <v>9.8500000000000004E-2</v>
       </c>
       <c r="K49" s="19">
-        <v>0.1754</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="14">
-        <v>7</v>
-      </c>
-      <c r="B50" s="19">
-        <v>0.1754</v>
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="L49" s="19">
+        <v>0.1754</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="14">
+        <v>7</v>
       </c>
       <c r="C50" s="19">
         <v>0.1754</v>
       </c>
       <c r="D50" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.1754</v>
       </c>
       <c r="E50" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="F50" s="19">
-        <v>0.2631</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="G50" s="19">
-        <v>0.13930000000000001</v>
+        <v>0.2631</v>
       </c>
       <c r="H50" s="19">
-        <v>0.3105</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="I50" s="19">
-        <v>0.1754</v>
+        <v>0.3105</v>
       </c>
       <c r="J50" s="19">
         <v>0.1754</v>
       </c>
       <c r="K50" s="19">
-        <v>5.67E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="15">
-        <v>7</v>
-      </c>
-      <c r="B51" s="19">
-        <v>0.3105</v>
+        <v>0.1754</v>
+      </c>
+      <c r="L50" s="19">
+        <v>5.67E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="15">
+        <v>7</v>
       </c>
       <c r="C51" s="19">
-        <v>0.2036</v>
+        <v>0.3105</v>
       </c>
       <c r="D51" s="19">
         <v>0.2036</v>
@@ -2437,33 +2732,36 @@
         <v>0.2036</v>
       </c>
       <c r="G51" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.2036</v>
       </c>
       <c r="H51" s="19">
-        <v>5.67E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="I51" s="19">
-        <v>9.8500000000000004E-2</v>
+        <v>5.67E-2</v>
       </c>
       <c r="J51" s="19">
         <v>9.8500000000000004E-2</v>
       </c>
       <c r="K51" s="19">
-        <v>0.2036</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="22" t="s">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="L51" s="19">
+        <v>0.2036</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A52" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="19">
-        <v>5.67E-2</v>
-      </c>
       <c r="C52" s="19">
-        <v>0.13930000000000001</v>
+        <v>5.67E-2</v>
       </c>
       <c r="D52" s="19">
-        <v>0.40539999999999998</v>
+        <v>0.13930000000000001</v>
       </c>
       <c r="E52" s="19">
         <v>0.40539999999999998</v>
@@ -2472,18 +2770,21 @@
         <v>0.40539999999999998</v>
       </c>
       <c r="G52" s="19">
-        <v>5.67E-2</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="H52" s="19">
-        <v>0.40539999999999998</v>
+        <v>5.67E-2</v>
       </c>
       <c r="I52" s="19">
         <v>0.40539999999999998</v>
       </c>
       <c r="J52" s="19">
-        <v>0.3105</v>
+        <v>0.40539999999999998</v>
       </c>
       <c r="K52" s="19">
+        <v>0.3105</v>
+      </c>
+      <c r="L52" s="19">
         <v>0.13930000000000001</v>
       </c>
     </row>
@@ -2510,13 +2811,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
-      <c r="B2" s="21"/>
+      <c r="B2" s="22"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2680,6 +2981,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013B620F01982514694878B55267266B0" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c024e8050b9bf00871c28df4e0c2326c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="882bdec5-c3ce-4705-9a84-58ed8ad203ea" xmlns:ns3="c6fe3531-949f-4c96-ac1d-b793c48e3f25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b87bd66fdc6a8cc420d7eafee76624a9" ns2:_="" ns3:_="">
     <xsd:import namespace="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
@@ -2894,22 +3210,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D0AC7F6-BBA9-4D4F-9602-79D3A370FFBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E57259E-309B-4436-AC0A-ED983DC13E22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{338034A7-D514-4A24-A53A-A06F44F9D0CD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2926,21 +3244,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E57259E-309B-4436-AC0A-ED983DC13E22}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D0AC7F6-BBA9-4D4F-9602-79D3A370FFBE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
clean the data and simplify the code
</commit_message>
<xml_diff>
--- a/Outbound.xlsx
+++ b/Outbound.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bff73b0ba30a6b9/Dokumen/College Files/OR/OR8/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bff73b0ba30a6b9/Dokumen/College Files/OR/OR8/OR8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="11_30EFB159AC1B5F3C0B675960D0F62E0BFB9F52F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{289E12BE-A3E2-41DF-AE7D-B86CD9D0E74F}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="11_30EFB159AC1B5F3C0B675960D0F62E0BFB9F52F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58D6CBAD-0A11-4CF3-A017-F1F4967F426A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="859" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,7 +406,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -460,12 +460,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -473,6 +467,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -492,10 +498,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -767,10 +769,10 @@
   <dimension ref="A1:S52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="9" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="9" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A52"/>
+      <selection pane="bottomRight" activeCell="P53" sqref="M1:P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -786,7 +788,7 @@
     <col min="10" max="10" width="12.453125" customWidth="1"/>
     <col min="11" max="11" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="6" customWidth="1"/>
     <col min="16" max="16" width="13.90625" customWidth="1"/>
   </cols>
@@ -828,9 +830,10 @@
       <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="M1" s="26"/>
     </row>
     <row r="2" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="13">
@@ -866,9 +869,10 @@
       <c r="L2" s="19">
         <v>0.40539999999999998</v>
       </c>
+      <c r="M2" s="27"/>
     </row>
     <row r="3" spans="1:19" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="14">
@@ -904,9 +908,10 @@
       <c r="L3" s="19">
         <v>5.67E-2</v>
       </c>
+      <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="14">
@@ -942,12 +947,13 @@
       <c r="L4" s="19">
         <v>5.67E-2</v>
       </c>
+      <c r="M4" s="26"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="9"/>
       <c r="S4" s="9"/>
     </row>
     <row r="5" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="14">
@@ -983,12 +989,13 @@
       <c r="L5" s="19">
         <v>0.2036</v>
       </c>
+      <c r="M5" s="26"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
     </row>
     <row r="6" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="14">
@@ -1024,12 +1031,13 @@
       <c r="L6" s="19">
         <v>0.2631</v>
       </c>
+      <c r="M6" s="26"/>
       <c r="Q6" s="10"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
     </row>
     <row r="7" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="14">
@@ -1065,12 +1073,13 @@
       <c r="L7" s="19">
         <v>0.1754</v>
       </c>
+      <c r="M7" s="26"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
     </row>
     <row r="8" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="14">
@@ -1106,12 +1115,13 @@
       <c r="L8" s="19">
         <v>0.2036</v>
       </c>
+      <c r="M8" s="26"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
     </row>
     <row r="9" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="14">
@@ -1147,12 +1157,13 @@
       <c r="L9" s="19">
         <v>0.1754</v>
       </c>
+      <c r="M9" s="26"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="9"/>
       <c r="S9" s="9"/>
     </row>
     <row r="10" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="14">
@@ -1188,12 +1199,13 @@
       <c r="L10" s="19">
         <v>0.13930000000000001</v>
       </c>
+      <c r="M10" s="26"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
     </row>
     <row r="11" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="14">
@@ -1229,9 +1241,10 @@
       <c r="L11" s="19">
         <v>5.67E-2</v>
       </c>
+      <c r="M11" s="26"/>
     </row>
     <row r="12" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="22" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="14">
@@ -1267,9 +1280,10 @@
       <c r="L12" s="19">
         <v>0.40539999999999998</v>
       </c>
+      <c r="M12" s="26"/>
     </row>
     <row r="13" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="22" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="14">
@@ -1305,9 +1319,10 @@
       <c r="L13" s="19">
         <v>0.13930000000000001</v>
       </c>
+      <c r="M13" s="26"/>
     </row>
     <row r="14" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="22" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="14">
@@ -1343,9 +1358,10 @@
       <c r="L14" s="19">
         <v>0.2631</v>
       </c>
+      <c r="M14" s="27"/>
     </row>
     <row r="15" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="14">
@@ -1383,7 +1399,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="22" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="14">
@@ -1419,9 +1435,10 @@
       <c r="L16" s="19">
         <v>9.8500000000000004E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="24" t="s">
+      <c r="M16" s="26"/>
+    </row>
+    <row r="17" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="14">
@@ -1457,9 +1474,10 @@
       <c r="L17" s="19">
         <v>5.67E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="24" t="s">
+      <c r="M17" s="26"/>
+    </row>
+    <row r="18" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="22" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="14">
@@ -1495,9 +1513,10 @@
       <c r="L18" s="19">
         <v>5.67E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="24" t="s">
+      <c r="M18" s="26"/>
+    </row>
+    <row r="19" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="22" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="14">
@@ -1533,9 +1552,10 @@
       <c r="L19" s="19">
         <v>0.13930000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="24" t="s">
+      <c r="M19" s="26"/>
+    </row>
+    <row r="20" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="14">
@@ -1571,9 +1591,10 @@
       <c r="L20" s="19">
         <v>0.2036</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="24" t="s">
+      <c r="M20" s="26"/>
+    </row>
+    <row r="21" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="14">
@@ -1609,9 +1630,10 @@
       <c r="L21" s="19">
         <v>0.13930000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="24" t="s">
+      <c r="M21" s="26"/>
+    </row>
+    <row r="22" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="14">
@@ -1647,9 +1669,10 @@
       <c r="L22" s="19">
         <v>0.40539999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="24" t="s">
+      <c r="M22" s="26"/>
+    </row>
+    <row r="23" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="22" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="14">
@@ -1685,9 +1708,10 @@
       <c r="L23" s="19">
         <v>0.1754</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="24" t="s">
+      <c r="M23" s="26"/>
+    </row>
+    <row r="24" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="22" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="14">
@@ -1723,9 +1747,10 @@
       <c r="L24" s="19">
         <v>0.2036</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="24" t="s">
+      <c r="M24" s="26"/>
+    </row>
+    <row r="25" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="22" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="14">
@@ -1761,9 +1786,10 @@
       <c r="L25" s="19">
         <v>5.67E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="24" t="s">
+      <c r="M25" s="26"/>
+    </row>
+    <row r="26" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="22" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="14">
@@ -1799,9 +1825,10 @@
       <c r="L26" s="19">
         <v>5.67E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="24" t="s">
+      <c r="M26" s="26"/>
+    </row>
+    <row r="27" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="14">
@@ -1837,9 +1864,10 @@
       <c r="L27" s="19">
         <v>0.40539999999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="24" t="s">
+      <c r="M27" s="26"/>
+    </row>
+    <row r="28" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="22" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="14">
@@ -1875,9 +1903,10 @@
       <c r="L28" s="19">
         <v>5.67E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="24" t="s">
+      <c r="M28" s="26"/>
+    </row>
+    <row r="29" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B29" s="14">
@@ -1913,9 +1942,10 @@
       <c r="L29" s="19">
         <v>0.2036</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="24" t="s">
+      <c r="M29" s="26"/>
+    </row>
+    <row r="30" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B30" s="14">
@@ -1951,9 +1981,10 @@
       <c r="L30" s="19">
         <v>0.13930000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="24" t="s">
+      <c r="M30" s="26"/>
+    </row>
+    <row r="31" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="22" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="14">
@@ -1989,9 +2020,10 @@
       <c r="L31" s="19">
         <v>0.2631</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="24" t="s">
+      <c r="M31" s="26"/>
+    </row>
+    <row r="32" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B32" s="14">
@@ -2027,9 +2059,10 @@
       <c r="L32" s="19">
         <v>0.2036</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="24" t="s">
+      <c r="M32" s="26"/>
+    </row>
+    <row r="33" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="22" t="s">
         <v>48</v>
       </c>
       <c r="B33" s="14">
@@ -2065,9 +2098,10 @@
       <c r="L33" s="19">
         <v>0.1754</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="24" t="s">
+      <c r="M33" s="26"/>
+    </row>
+    <row r="34" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B34" s="14">
@@ -2103,9 +2137,10 @@
       <c r="L34" s="19">
         <v>0.3105</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="24" t="s">
+      <c r="M34" s="26"/>
+    </row>
+    <row r="35" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="22" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="14">
@@ -2141,9 +2176,10 @@
       <c r="L35" s="19">
         <v>0.2631</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="24" t="s">
+      <c r="M35" s="26"/>
+    </row>
+    <row r="36" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="22" t="s">
         <v>50</v>
       </c>
       <c r="B36" s="14">
@@ -2179,9 +2215,10 @@
       <c r="L36" s="19">
         <v>9.8500000000000004E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="24" t="s">
+      <c r="M36" s="26"/>
+    </row>
+    <row r="37" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="22" t="s">
         <v>51</v>
       </c>
       <c r="B37" s="14">
@@ -2217,9 +2254,10 @@
       <c r="L37" s="19">
         <v>9.8500000000000004E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="24" t="s">
+      <c r="M37" s="26"/>
+    </row>
+    <row r="38" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B38" s="14">
@@ -2255,9 +2293,10 @@
       <c r="L38" s="19">
         <v>0.40539999999999998</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="24" t="s">
+      <c r="M38" s="27"/>
+    </row>
+    <row r="39" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="22" t="s">
         <v>3</v>
       </c>
       <c r="B39" s="14">
@@ -2294,8 +2333,8 @@
         <v>0.13930000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="24" t="s">
+    <row r="40" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B40" s="14">
@@ -2331,9 +2370,10 @@
       <c r="L40" s="19">
         <v>0.2036</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="24" t="s">
+      <c r="M40" s="26"/>
+    </row>
+    <row r="41" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="22" t="s">
         <v>54</v>
       </c>
       <c r="B41" s="14">
@@ -2369,9 +2409,10 @@
       <c r="L41" s="19">
         <v>5.67E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="24" t="s">
+      <c r="M41" s="26"/>
+    </row>
+    <row r="42" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B42" s="14">
@@ -2407,9 +2448,10 @@
       <c r="L42" s="19">
         <v>0.1754</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="24" t="s">
+      <c r="M42" s="26"/>
+    </row>
+    <row r="43" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A43" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B43" s="14">
@@ -2445,9 +2487,10 @@
       <c r="L43" s="19">
         <v>9.8500000000000004E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="24" t="s">
+      <c r="M43" s="26"/>
+    </row>
+    <row r="44" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A44" s="22" t="s">
         <v>2</v>
       </c>
       <c r="B44" s="14">
@@ -2483,9 +2526,10 @@
       <c r="L44" s="19">
         <v>0.13930000000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="24" t="s">
+      <c r="M44" s="26"/>
+    </row>
+    <row r="45" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A45" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B45" s="14">
@@ -2521,9 +2565,10 @@
       <c r="L45" s="19">
         <v>0.13930000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="24" t="s">
+      <c r="M45" s="26"/>
+    </row>
+    <row r="46" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A46" s="22" t="s">
         <v>56</v>
       </c>
       <c r="B46" s="14">
@@ -2559,9 +2604,10 @@
       <c r="L46" s="19">
         <v>5.67E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A47" s="24" t="s">
+      <c r="M46" s="26"/>
+    </row>
+    <row r="47" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A47" s="22" t="s">
         <v>57</v>
       </c>
       <c r="B47" s="14">
@@ -2597,9 +2643,10 @@
       <c r="L47" s="19">
         <v>0.3105</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="24" t="s">
+      <c r="M47" s="26"/>
+    </row>
+    <row r="48" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A48" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B48" s="14">
@@ -2635,9 +2682,10 @@
       <c r="L48" s="19">
         <v>0.40539999999999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="24" t="s">
+      <c r="M48" s="27"/>
+    </row>
+    <row r="49" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="22" t="s">
         <v>58</v>
       </c>
       <c r="B49" s="14">
@@ -2674,8 +2722,8 @@
         <v>0.1754</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A50" s="24" t="s">
+    <row r="50" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A50" s="22" t="s">
         <v>59</v>
       </c>
       <c r="B50" s="14">
@@ -2711,9 +2759,10 @@
       <c r="L50" s="19">
         <v>5.67E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="25" t="s">
+      <c r="M50" s="26"/>
+    </row>
+    <row r="51" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A51" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B51" s="15">
@@ -2749,8 +2798,9 @@
       <c r="L51" s="19">
         <v>0.2036</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="M51" s="26"/>
+    </row>
+    <row r="52" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
         <v>61</v>
       </c>
@@ -2787,6 +2837,7 @@
       <c r="L52" s="19">
         <v>0.13930000000000001</v>
       </c>
+      <c r="M52" s="26"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2811,13 +2862,13 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="24" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
-      <c r="B2" s="22"/>
+      <c r="B2" s="25"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2981,21 +3032,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013B620F01982514694878B55267266B0" ma:contentTypeVersion="13" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c024e8050b9bf00871c28df4e0c2326c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="882bdec5-c3ce-4705-9a84-58ed8ad203ea" xmlns:ns3="c6fe3531-949f-4c96-ac1d-b793c48e3f25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b87bd66fdc6a8cc420d7eafee76624a9" ns2:_="" ns3:_="">
     <xsd:import namespace="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
@@ -3210,24 +3246,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D0AC7F6-BBA9-4D4F-9602-79D3A370FFBE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E57259E-309B-4436-AC0A-ED983DC13E22}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{338034A7-D514-4A24-A53A-A06F44F9D0CD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3244,4 +3278,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E57259E-309B-4436-AC0A-ED983DC13E22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D0AC7F6-BBA9-4D4F-9602-79D3A370FFBE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>